<commit_message>
Add chi^2 statistical comparison
</commit_message>
<xml_diff>
--- a/paper_tables.xlsx
+++ b/paper_tables.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colby\Documents\GitHub\pfHRP_MLModel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colbyford/Documents/pfHRP_MLModel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5758452-4FC2-4AF7-AADF-00058712A9C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17EF5DA-F418-0043-ADAF-C0A998BE0B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14175" yWindow="3495" windowWidth="18120" windowHeight="12630" firstSheet="1" activeTab="2" xr2:uid="{90FC2CFC-1E1B-44CB-A48A-2F387CB992ED}"/>
+    <workbookView xWindow="1800" yWindow="1460" windowWidth="25140" windowHeight="12640" firstSheet="1" activeTab="3" xr2:uid="{90FC2CFC-1E1B-44CB-A48A-2F387CB992ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Model Metrics" sheetId="1" r:id="rId1"/>
     <sheet name="Type Prevalence by Loc" sheetId="2" r:id="rId2"/>
     <sheet name="DNA - Test Matches" sheetId="3" r:id="rId3"/>
-    <sheet name="RDTqPCR Confustion Matrix" sheetId="4" r:id="rId4"/>
+    <sheet name="chi-sq" sheetId="5" r:id="rId4"/>
+    <sheet name="RDTqPCR Confustion Matrix" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="154">
   <si>
     <t>Precision</t>
   </si>
@@ -432,6 +433,90 @@
   </si>
   <si>
     <t>F1 Score</t>
+  </si>
+  <si>
+    <t>Voting Ensemble
+Types 2 and 7</t>
+  </si>
+  <si>
+    <t>Extreme Random Trees
+Types 2 and 7</t>
+  </si>
+  <si>
+    <t>Extreme Random Trees
+Types 3 and 5 and 10</t>
+  </si>
+  <si>
+    <t>Voting Ensemble
+Types 3 and 5 and 10</t>
+  </si>
+  <si>
+    <t>Extreme Random Trees
+Types 1 thru 24</t>
+  </si>
+  <si>
+    <t>Voting Ensemble
+Types 1 thru 24</t>
+  </si>
+  <si>
+    <t>32.668
+(1.093e-08)</t>
+  </si>
+  <si>
+    <t>67
+(2.715e-16)</t>
+  </si>
+  <si>
+    <t>7.1373
+(0.00755)</t>
+  </si>
+  <si>
+    <t>3.1485
+(0.076)</t>
+  </si>
+  <si>
+    <t>8.963
+(0.002755)</t>
+  </si>
+  <si>
+    <t>9.9844
+(0.001579)</t>
+  </si>
+  <si>
+    <t>11.981
+(0.0005375)</t>
+  </si>
+  <si>
+    <t>10.073
+(0.001505)</t>
+  </si>
+  <si>
+    <t>10.338
+(0.001303)</t>
+  </si>
+  <si>
+    <t>10.866
+(0.0009797)</t>
+  </si>
+  <si>
+    <t>12.55
+(0.0003962)</t>
+  </si>
+  <si>
+    <t>15.5
+(8.249e-05)</t>
+  </si>
+  <si>
+    <t>Types 2 and 7</t>
+  </si>
+  <si>
+    <t>Types 1 thru 24</t>
+  </si>
+  <si>
+    <t>Types 3 and 5 and 10</t>
+  </si>
+  <si>
+    <t>ML</t>
   </si>
 </sst>
 </file>
@@ -484,7 +569,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -495,6 +580,15 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -817,14 +911,14 @@
       <selection activeCell="B1" sqref="B1:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -850,11 +944,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -876,9 +970,9 @@
         <v>0.64136000000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
       <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
@@ -898,9 +992,9 @@
         <v>0.64136000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -922,9 +1016,9 @@
         <v>0.79981999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
       <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
@@ -944,9 +1038,9 @@
         <v>0.79981999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -968,9 +1062,9 @@
         <v>0.82838999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
       <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1011,9 +1105,9 @@
       <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1033,7 +1127,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1053,7 +1147,7 @@
         <v>0.9509803921568627</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1073,7 +1167,7 @@
         <v>0.92156862745098034</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1093,7 +1187,7 @@
         <v>0.6470588235294118</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1113,7 +1207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1133,7 +1227,7 @@
         <v>0.55882352941176472</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1153,7 +1247,7 @@
         <v>0.92156862745098034</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1173,7 +1267,7 @@
         <v>0.9509803921568627</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1193,7 +1287,7 @@
         <v>0.78431372549019607</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1213,7 +1307,7 @@
         <v>0.78431372549019607</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1233,7 +1327,7 @@
         <v>0.69607843137254899</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1253,7 +1347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1273,7 +1367,7 @@
         <v>0.20588235294117646</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1293,7 +1387,7 @@
         <v>0.57843137254901966</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1313,7 +1407,7 @@
         <v>8.8235294117647065E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1333,7 +1427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1353,7 +1447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1373,7 +1467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1393,7 +1487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1413,7 +1507,7 @@
         <v>0.97058823529411764</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1433,7 +1527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1453,7 +1547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1473,7 +1567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1493,7 +1587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1522,13 +1616,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48A2570E-2E87-432E-894F-42B5D3587C38}">
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -1551,7 +1645,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -1568,7 +1662,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1585,7 +1679,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1608,7 +1702,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1631,7 +1725,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1654,7 +1748,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1677,7 +1771,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1694,7 +1788,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -1717,7 +1811,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -1734,7 +1828,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -1757,7 +1851,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -1774,7 +1868,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -1797,7 +1891,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -1820,7 +1914,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -1837,7 +1931,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -1860,7 +1954,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -1883,7 +1977,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -1906,7 +2000,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -1929,7 +2023,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>44</v>
       </c>
@@ -1952,7 +2046,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -1975,7 +2069,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -1992,7 +2086,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>47</v>
       </c>
@@ -2015,7 +2109,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -2032,7 +2126,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>49</v>
       </c>
@@ -2049,7 +2143,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -2072,7 +2166,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -2095,7 +2189,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -2112,7 +2206,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>53</v>
       </c>
@@ -2129,7 +2223,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>54</v>
       </c>
@@ -2152,7 +2246,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>55</v>
       </c>
@@ -2175,7 +2269,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>56</v>
       </c>
@@ -2198,7 +2292,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>57</v>
       </c>
@@ -2221,7 +2315,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>58</v>
       </c>
@@ -2244,7 +2338,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>59</v>
       </c>
@@ -2261,7 +2355,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>60</v>
       </c>
@@ -2284,7 +2378,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>61</v>
       </c>
@@ -2301,7 +2395,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>62</v>
       </c>
@@ -2318,7 +2412,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>63</v>
       </c>
@@ -2335,7 +2429,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>64</v>
       </c>
@@ -2352,7 +2446,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>65</v>
       </c>
@@ -2375,7 +2469,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>66</v>
       </c>
@@ -2398,7 +2492,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>67</v>
       </c>
@@ -2421,7 +2515,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>68</v>
       </c>
@@ -2438,7 +2532,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>69</v>
       </c>
@@ -2461,7 +2555,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>70</v>
       </c>
@@ -2484,7 +2578,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>71</v>
       </c>
@@ -2507,7 +2601,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>72</v>
       </c>
@@ -2530,7 +2624,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>73</v>
       </c>
@@ -2553,7 +2647,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>74</v>
       </c>
@@ -2576,7 +2670,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>75</v>
       </c>
@@ -2599,7 +2693,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>76</v>
       </c>
@@ -2622,7 +2716,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>77</v>
       </c>
@@ -2639,7 +2733,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>78</v>
       </c>
@@ -2662,7 +2756,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>79</v>
       </c>
@@ -2685,7 +2779,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>80</v>
       </c>
@@ -2708,7 +2802,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>81</v>
       </c>
@@ -2725,7 +2819,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>82</v>
       </c>
@@ -2742,7 +2836,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>83</v>
       </c>
@@ -2759,7 +2853,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>84</v>
       </c>
@@ -2782,7 +2876,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>85</v>
       </c>
@@ -2799,7 +2893,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>86</v>
       </c>
@@ -2816,7 +2910,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>87</v>
       </c>
@@ -2839,7 +2933,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>88</v>
       </c>
@@ -2856,7 +2950,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>89</v>
       </c>
@@ -2873,7 +2967,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>90</v>
       </c>
@@ -2896,7 +2990,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>91</v>
       </c>
@@ -2913,7 +3007,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>92</v>
       </c>
@@ -2930,7 +3024,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>93</v>
       </c>
@@ -2947,7 +3041,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>94</v>
       </c>
@@ -2970,7 +3064,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>95</v>
       </c>
@@ -2987,7 +3081,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>96</v>
       </c>
@@ -3010,7 +3104,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>97</v>
       </c>
@@ -3033,7 +3127,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>98</v>
       </c>
@@ -3050,7 +3144,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>99</v>
       </c>
@@ -3073,7 +3167,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>100</v>
       </c>
@@ -3090,7 +3184,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>101</v>
       </c>
@@ -3113,7 +3207,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>102</v>
       </c>
@@ -3136,7 +3230,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>103</v>
       </c>
@@ -3159,7 +3253,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>104</v>
       </c>
@@ -3182,7 +3276,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>105</v>
       </c>
@@ -3205,7 +3299,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>106</v>
       </c>
@@ -3228,7 +3322,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>107</v>
       </c>
@@ -3251,7 +3345,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>108</v>
       </c>
@@ -3274,7 +3368,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>109</v>
       </c>
@@ -3297,7 +3391,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>110</v>
       </c>
@@ -3320,7 +3414,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>111</v>
       </c>
@@ -3343,7 +3437,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>112</v>
       </c>
@@ -3360,7 +3454,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>113</v>
       </c>
@@ -3383,7 +3477,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>114</v>
       </c>
@@ -3406,7 +3500,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>115</v>
       </c>
@@ -3429,7 +3523,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>116</v>
       </c>
@@ -3452,7 +3546,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>117</v>
       </c>
@@ -3475,7 +3569,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>118</v>
       </c>
@@ -3498,7 +3592,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>119</v>
       </c>
@@ -3515,7 +3609,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>120</v>
       </c>
@@ -3532,7 +3626,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>121</v>
       </c>
@@ -3549,7 +3643,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>122</v>
       </c>
@@ -3566,7 +3660,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>123</v>
       </c>
@@ -3589,7 +3683,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>124</v>
       </c>
@@ -3612,7 +3706,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>125</v>
       </c>
@@ -3635,6 +3729,184 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4654D2EA-4378-564E-B113-E4E8F742E7AB}">
+  <dimension ref="A1:I14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="23.1640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="16.5" style="4" customWidth="1"/>
+    <col min="7" max="7" width="23.33203125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="24.1640625" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="B1" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B8" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C9" s="7"/>
+    </row>
+    <row r="10" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="6"/>
+      <c r="C14" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B8:C8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{260C20C9-786A-4054-90F3-8E11C8948E08}">
   <dimension ref="A1:D12"/>
   <sheetViews>
@@ -3642,20 +3914,20 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>128</v>
       </c>
@@ -3669,7 +3941,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3683,7 +3955,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3697,7 +3969,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>126</v>
       </c>
@@ -3711,7 +3983,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -3720,7 +3992,7 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>129</v>
       </c>
@@ -3729,7 +4001,7 @@
         <v>0.83783783783783783</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>130</v>
       </c>
@@ -3738,7 +4010,7 @@
         <v>0.84615384615384615</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>131</v>
       </c>

</xml_diff>